<commit_message>
added all skills, make pie chart sample
</commit_message>
<xml_diff>
--- a/Naukricom.xlsx
+++ b/Naukricom.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,20 +446,25 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Skills</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Location</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>experience</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>salary</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
@@ -471,32 +476,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Android Application Developer</t>
+          <t>Computer Science Engineering- Professor</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Quick Infotech</t>
+          <t>Sharda University3.6248  Reviews</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Lucknow</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, advisory, computer</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0-1 Yrs</t>
+          <t>Greater Noida</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>10-12 Yrs</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Deep knowledge of Android automation and unit testing frameworks . Ability to lead and ...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>experience as a Professor including 5 years of administrative experience in a reputed U...</t>
         </is>
       </c>
     </row>
@@ -506,32 +516,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Senior Software Engineer</t>
+          <t>Computer Science &amp; Informatics- Professor</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BNP Paribas3.91087  Reviews</t>
+          <t>Maharshi Dayanand University (MDU)4.819  Reviews</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, Education, Computer</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0-3 Yrs</t>
+          <t>Jaipur</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>7-10 Yrs</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>. First class Graduate in any discipline (Computer Science preferred) from a reputed Un...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Work with students who are studying for a degree or a certificate or certification or a...</t>
         </is>
       </c>
     </row>
@@ -541,32 +556,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Trainee Software Engineer</t>
+          <t>Computer Science &amp; Informatics- Professor</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Helios Web4.87  Reviews</t>
+          <t>Maharshi Dayanand University (MDU)4.819  Reviews</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, Education, Computer</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Jaipur</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>0-1 Yrs</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>8-11 Yrs</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Experience - 0 - 1 yrs . . Requirement . . MCA or BE / BTech in Computer Science, Compu...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Work with students who are studying for a degree or a certificate or certification or a...</t>
         </is>
       </c>
     </row>
@@ -576,32 +596,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Requirement of Software Developer Fresher</t>
+          <t>Sr . Software Developer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ujobs Consulting</t>
+          <t>Newstar Infotech</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Remote</t>
+          <t>Computer science, Web technologies, SQL database, Programming, Database, Application software, IOS, DBMS</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0-0 Yrs</t>
+          <t>Ahmedabad</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>0-1 Yrs</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Hiring Freshers (BCA/MCA/BTech 2022, 2023, 2024) Candidate required to interface with p...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Bachelor s degree or equivalent experience in Computer Science or related field Develop...</t>
         </is>
       </c>
     </row>
@@ -611,32 +636,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Software Development Engineer (SDE-1) / Full Stack Developer</t>
+          <t>Software Developer</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>One Muthoot</t>
+          <t>Hi Tech3.8135  Reviews</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Bangalore/Bengaluru</t>
+          <t>C++, development, software, Development Manager, AutoCAD, VC++, CAD, Program Executive</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0-2 Yrs</t>
+          <t>Chennai</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>0-1 Yrs</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>. You should have knowledge and experience in Front End technologies . You should have ...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>- Must be ambitious and have a desire to learn new skills</t>
         </is>
       </c>
     </row>
@@ -646,32 +676,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Software Engineer - Fullstack Developer</t>
+          <t>Computer Science Faculty</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Siemens4.24020  Reviews</t>
+          <t>Amity University3.6966  Reviews</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Computer Science, Information Technology, Science, Technology, Computer</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0-5 Yrs</t>
+          <t>Mohali, Punjab</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>3-8 Yrs</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Bachelor s degree in Computer Science, Information Systems, orequivalent education or w...</t>
+          <t>1.5-6 Lacs PA</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Teaching: Provide high-quality instruction at the undergraduate level, ensuring course ...</t>
         </is>
       </c>
     </row>
@@ -681,32 +716,37 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>Computer Science- TGT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Adroit Solutions3.914  Reviews</t>
+          <t>DPS Gandhinagar3.91694  Reviews</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Chennai</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, advisory, tgt</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0-1 Yrs</t>
+          <t>Gandhinagar</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>3-6 Yrs</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Minimum an IT related Degree MCA or BTech or BEOther skills required - Must have some e...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Job Description: ? Must possess a B.Ed. degree from recognized institution ? Schooling ...</t>
         </is>
       </c>
     </row>
@@ -716,32 +756,37 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Software Developer</t>
+          <t>Computer Science - PGT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Finedge3.035  Reviews</t>
+          <t>DPS Patna3.91694  Reviews</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Gurgaon/Gurugram</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, advisory, computer</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0-2 Yrs</t>
+          <t>Patna</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>4-6 Yrs</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Past experience in developing systems for the Financial Services industry would be an a...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Job Description: ? Must possess a B.Ed. degree from recognized institution ? Schooling ...</t>
         </is>
       </c>
     </row>
@@ -751,32 +796,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Embedded Software Developer</t>
+          <t>Computer Science Faculty</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Embed Square Solutions4.04  Reviews</t>
+          <t>Aditya P.U. College</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Pune</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, Training, Science</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0-3 Yrs</t>
+          <t>Bangalore/Bengaluru</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>1-3 Yrs</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Bachelors or Masters degree in Computer Science, Electrical Engineering, or related fie...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Key responsibilities of the job include: ? providing support to children in reading and...</t>
         </is>
       </c>
     </row>
@@ -786,32 +836,37 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jr. Software Developer</t>
+          <t>TGT Computer Science</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>D Source</t>
+          <t>Zydus School For Excellence4.112  Reviews</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Nasik/Nashik</t>
+          <t>Professor, Tutor, English, Teachers, Education, Trainer, Lecturer, Teaching</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0-2 Yrs</t>
+          <t>Godhavi</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>3-5 Yrs</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Good programming and logical skills Good understanding of Client-side scripting / JavaS...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Develop and maintain good Working habits and discipline in classroomsRequired TGT Compu...</t>
         </is>
       </c>
     </row>
@@ -821,32 +876,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Software Developers</t>
+          <t>Professor - Computer Science</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>IT Bytes5.04  Reviews</t>
+          <t>Flame University4.621  Reviews</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dehradun</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, computer, computer science</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0-1 Yrs</t>
+          <t>Bengaluru</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>10-13 Yrs</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Software developers required with 0 to 1 year of experiece. Requirements Qualifications...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Work with students who are studying for a degree or a certificate or certification or a...</t>
         </is>
       </c>
     </row>
@@ -856,32 +916,37 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Associate Software Developer</t>
+          <t>Computer Science - Professor</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>My Virtual Teams4.39  Reviews</t>
+          <t>R. K. C. S. Educational Society</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ludhiana</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, advisory, computer</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0-5 Yrs</t>
+          <t>Firozabad</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>10-12 Yrs</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Job description . We are seeking a talented and passionate Fresher Web Developer to joi...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>A minimum of ten years of teaching experience in university / college, and / or experie...</t>
         </is>
       </c>
     </row>
@@ -891,32 +956,37 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Computer Science Teacher (Grade 11th &amp; 12th)</t>
+          <t>Computer Science - Professor</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Educohire3.55  Reviews</t>
+          <t>R. K. C. S. Educational Society</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Ahmedabad</t>
+          <t>Counselor, Mentor, Trainer, Advisor, Educator, Teaching, advisory, computer</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2-5 Yrs</t>
+          <t>New Delhi</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>10-15 Yrs</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Education and Qualifications:Obtain a bachelors or masters degree in computer science, ...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>A minimum of ten years of teaching experience in university / college, and / or experie...</t>
         </is>
       </c>
     </row>
@@ -926,32 +996,37 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>PGT TGT Computer Science</t>
+          <t>Software Application Developer (OST)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Digiimento Educational Services</t>
+          <t>Logonb2b</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Kolkata, Mumbai, New Delhi, Hyderabad/Secunderabad, Pune, Chennai, Bangalore/Bengaluru</t>
+          <t>software, E-commerce, HTML, Research, Information technology, Joomla, Computer science, application</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4-10 Yrs</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>0-2 Yrs</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Curriculum Development: Create and develop instructional materials and lesson plans t...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Software Application Developer (OST) Skill: Good research, analytical, and Communicatio...</t>
         </is>
       </c>
     </row>
@@ -961,32 +1036,37 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>TGT &amp; PGT (Computer Science), AI, Web Technology</t>
+          <t>Windows Application Software Developer</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NH Goel World School4.221  Reviews</t>
+          <t>Bluesurf Engineering Solutions</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Raipur</t>
+          <t>Computer science, Agile scrum, Windows application, devops, Electronics, Telecommunication, Instrumentation, Application development</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2-6 Yrs</t>
+          <t>Pune</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>0-1 Yrs</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Qualifications and Skills:Bachelors / Masters degree in Computer Science, AI, Web Techn...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Bachelor s or master s degree in computer science / IT / Electronics / Electronics Tele...</t>
         </is>
       </c>
     </row>
@@ -996,32 +1076,37 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Middle School Computer Science Teacher</t>
+          <t>computer science Teacher AI, Machine Learning</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Teacher Pool</t>
+          <t>BDS Consultancy</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bangalore/Bengaluru</t>
+          <t>Computer Science, machine learning, ai, web development, cloud computing, Teaching, Computer, Machine</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1-5 Yrs</t>
+          <t>Kolkata, West Bengal</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Not disclosed</t>
+          <t>3-8 Yrs</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Qualifications: . A bachelors degree in computer science or a related field a masters d...</t>
+          <t>5-7.5 Lacs PA</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>The candidate should have ME / M.Tech, Ph.D / Doctorate in Computer Science (Image Proc...</t>
         </is>
       </c>
     </row>
@@ -1031,32 +1116,37 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PRT/TGT Computer Science Teacher</t>
+          <t>Computer Science Faculty</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Shiksha Valley School3.514  Reviews</t>
+          <t>Vision Group of Colleges</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Dibrugarh, Assam</t>
+          <t>Computer Teaching, Lecturer Activities, Professor Activities, Education, Computer Science, Teaching, Information Technology, Computer</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3-6 Yrs</t>
+          <t>Chittaurgarh, Rajasthan</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1.5-4.25 Lacs PA</t>
+          <t>1-2 Yrs</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Minimum experience of 3 years or more in a CBSE affiliated SchoolGraduate/ Post Graduat...</t>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Deliver lectures, conduct practical sessions, and facilitate discussions for BCA (Bache...</t>
         </is>
       </c>
     </row>
@@ -1066,32 +1156,117 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hiring For TGT &amp; PGT Computer Science</t>
+          <t>Computer Science Faculty</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Alpine Convent School3.349  Reviews</t>
+          <t>Gnana Jyothi School3.03  Reviews</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Gurgaon/ Gurugram, Haryana</t>
+          <t>Spoken English, Doctoral degree in computer science or a related field Minimum of five years of experience working in software development, Computer, English, Development, Computer science, Degree In Computer Science, Software</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1-3 Yrs</t>
+          <t>Tumkur, Mysore/Mysuru, Bangalore/Bengaluru(Bagalur +2)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>4-6 Lacs PA</t>
+          <t>3-5 Yrs</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Alpine Convent School is hiring highly experienced TGT &amp; PGT Computer Science with exce...</t>
+          <t>3-4 Lacs PA</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Instruct students on how computers work, including the basic science and mathematics be...</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Professor -  Computer Science &amp; Engineering</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sambhram Institute Of Technology2.916  Reviews</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Professor, Tutor, Teachers, Education, Trainer, Lecturer, Computer Science &amp; Engineering, Teaching</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bengaluru, Bangalore</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>8-10 Yrs</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Required Professor for Computer Science &amp; Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Computer science Engineer - BHEL Jobs</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Right Step Consulting</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Software design, Programming, Software, TelecomDebugging, Application software, Linux kernelComp, Engineering, Computer science</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Noida</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1-5 Yrs</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Industry: Semiconductors / Electronics . Functional Area: IT Software - Telecom Softwar...</t>
         </is>
       </c>
     </row>

</xml_diff>